<commit_message>
finish demo bact abundance data
</commit_message>
<xml_diff>
--- a/Input_Data/week3/ACIDD_Exp_BactAbund.xlsx
+++ b/Input_Data/week3/ACIDD_Exp_BactAbund.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasbaetge/GITHUB/eemb144l/Input_Data/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4B60BA-3045-A54B-9013-4A60A277FAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58C4B1C-C5E9-6643-BD8F-A6F70E5406E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="3440" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{DFE3F779-83E5-5C45-8A1C-F78D6D093241}"/>
+    <workbookView xWindow="18400" yWindow="3440" windowWidth="26840" windowHeight="15940" xr2:uid="{DFE3F779-83E5-5C45-8A1C-F78D6D093241}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Ash</t>
   </si>
   <si>
     <t>D</t>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>Datetime</t>
+  </si>
+  <si>
+    <t>Ash Leachate</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0444EC-73B7-544C-8786-238F0C09BB54}">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,13 +552,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -570,34 +570,34 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
       <c r="K1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
         <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -605,7 +605,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -632,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -658,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -711,7 +711,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -764,7 +764,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -791,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -844,7 +844,7 @@
         <v>4</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" t="b">
         <v>0</v>
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -897,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -1003,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
@@ -1029,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>15</v>
@@ -1056,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>15</v>
@@ -1109,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" t="b">
         <v>1</v>
@@ -1135,7 +1135,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -1162,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" t="b">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -1215,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" t="b">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -1268,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
@@ -1294,7 +1294,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -1321,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
@@ -1347,7 +1347,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1374,7 +1374,7 @@
         <v>4</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L16" t="b">
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>15</v>
@@ -1427,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L17" t="b">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L18" t="b">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>15</v>
@@ -1533,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -1559,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>15</v>
@@ -1586,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -1639,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L21" t="b">
         <v>0</v>
@@ -1665,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -1692,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -1718,7 +1718,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -1745,7 +1745,7 @@
         <v>4</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L23" t="b">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1798,7 +1798,7 @@
         <v>4</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
@@ -1824,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -1851,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" t="b">
         <v>0</v>
@@ -1877,7 +1877,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26">
         <v>15</v>
@@ -1892,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -1904,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L26" t="b">
         <v>0</v>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -1945,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H27">
         <v>10</v>
@@ -1957,7 +1957,7 @@
         <v>4</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L27" t="b">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -1998,7 +1998,7 @@
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H28">
         <v>10</v>
@@ -2010,7 +2010,7 @@
         <v>4</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L28" t="b">
         <v>0</v>
@@ -2036,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>15</v>
@@ -2051,7 +2051,7 @@
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -2063,7 +2063,7 @@
         <v>4</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L29" t="b">
         <v>0</v>
@@ -2089,7 +2089,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>15</v>
@@ -2104,7 +2104,7 @@
         <v>6</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -2116,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L30" t="b">
         <v>0</v>
@@ -2142,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>15</v>
@@ -2157,7 +2157,7 @@
         <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H31">
         <v>10</v>
@@ -2169,7 +2169,7 @@
         <v>4</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L31" t="b">
         <v>1</v>
@@ -2195,7 +2195,7 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>15</v>
@@ -2210,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H32">
         <v>10</v>
@@ -2222,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L32" t="b">
         <v>0</v>
@@ -2248,7 +2248,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>15</v>
@@ -2263,7 +2263,7 @@
         <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H33">
         <v>10</v>
@@ -2275,7 +2275,7 @@
         <v>4</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L33" t="b">
         <v>1</v>
@@ -2301,7 +2301,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34">
         <v>15</v>
@@ -2316,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H34">
         <v>10</v>
@@ -2328,7 +2328,7 @@
         <v>4</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
@@ -2354,7 +2354,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35">
         <v>15</v>
@@ -2363,13 +2363,13 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H35">
         <v>10</v>
@@ -2381,7 +2381,7 @@
         <v>4</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L35" t="b">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36">
         <v>15</v>
@@ -2416,13 +2416,13 @@
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H36">
         <v>10</v>
@@ -2434,7 +2434,7 @@
         <v>4</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
@@ -2460,7 +2460,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>15</v>
@@ -2469,13 +2469,13 @@
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H37">
         <v>10</v>
@@ -2487,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L37" t="b">
         <v>0</v>
@@ -2513,7 +2513,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38">
         <v>15</v>
@@ -2522,13 +2522,13 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38">
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H38">
         <v>10</v>
@@ -2540,7 +2540,7 @@
         <v>4</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
@@ -2566,7 +2566,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39">
         <v>15</v>
@@ -2575,13 +2575,13 @@
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39">
         <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H39">
         <v>10</v>
@@ -2593,7 +2593,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
@@ -2619,7 +2619,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40">
         <v>15</v>
@@ -2628,13 +2628,13 @@
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40">
         <v>5</v>
       </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H40">
         <v>10</v>
@@ -2646,7 +2646,7 @@
         <v>4</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L40" t="b">
         <v>0</v>
@@ -2672,7 +2672,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41">
         <v>15</v>
@@ -2681,13 +2681,13 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41">
         <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -2699,7 +2699,7 @@
         <v>4</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
@@ -2725,7 +2725,7 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42">
         <v>15</v>
@@ -2734,13 +2734,13 @@
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H42">
         <v>10</v>
@@ -2752,7 +2752,7 @@
         <v>4</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
@@ -2778,7 +2778,7 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>15</v>
@@ -2787,13 +2787,13 @@
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H43">
         <v>10</v>
@@ -2805,7 +2805,7 @@
         <v>4</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L43" t="b">
         <v>0</v>
@@ -2831,7 +2831,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44">
         <v>15</v>
@@ -2840,13 +2840,13 @@
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H44">
         <v>10</v>
@@ -2858,7 +2858,7 @@
         <v>4</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L44" t="b">
         <v>1</v>
@@ -2884,7 +2884,7 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45">
         <v>15</v>
@@ -2893,13 +2893,13 @@
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45">
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H45">
         <v>10</v>
@@ -2911,7 +2911,7 @@
         <v>4</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L45" t="b">
         <v>0</v>
@@ -2934,10 +2934,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C46">
         <v>15</v>
@@ -2964,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L46" t="b">
         <v>1</v>
@@ -2987,10 +2987,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -3017,7 +3017,7 @@
         <v>4</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
@@ -3040,10 +3040,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C48">
         <v>15</v>
@@ -3070,7 +3070,7 @@
         <v>4</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L48" t="b">
         <v>0</v>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -3123,7 +3123,7 @@
         <v>4</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L49" t="b">
         <v>0</v>
@@ -3146,10 +3146,10 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C50">
         <v>15</v>
@@ -3176,7 +3176,7 @@
         <v>4</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L50" t="b">
         <v>0</v>
@@ -3199,10 +3199,10 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C51">
         <v>15</v>
@@ -3229,7 +3229,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L51" t="b">
         <v>0</v>
@@ -3252,10 +3252,10 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C52">
         <v>15</v>
@@ -3282,7 +3282,7 @@
         <v>4</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L52" t="b">
         <v>1</v>
@@ -3305,10 +3305,10 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C53">
         <v>15</v>
@@ -3335,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L53" t="b">
         <v>0</v>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>15</v>
@@ -3388,7 +3388,7 @@
         <v>4</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L54" t="b">
         <v>0</v>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55">
         <v>15</v>
@@ -3441,7 +3441,7 @@
         <v>4</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L55" t="b">
         <v>0</v>
@@ -3464,10 +3464,10 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56">
         <v>15</v>
@@ -3494,7 +3494,7 @@
         <v>4</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L56" t="b">
         <v>1</v>
@@ -3517,10 +3517,10 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57">
         <v>15</v>
@@ -3547,7 +3547,7 @@
         <v>4</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L57" t="b">
         <v>0</v>
@@ -3570,10 +3570,10 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C58">
         <v>15</v>
@@ -3600,7 +3600,7 @@
         <v>4</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L58" t="b">
         <v>0</v>
@@ -3623,10 +3623,10 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C59">
         <v>15</v>
@@ -3653,7 +3653,7 @@
         <v>4</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L59" t="b">
         <v>0</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C60">
         <v>15</v>
@@ -3706,7 +3706,7 @@
         <v>4</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L60" t="b">
         <v>0</v>
@@ -3729,10 +3729,10 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61">
         <v>15</v>
@@ -3759,7 +3759,7 @@
         <v>4</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L61" t="b">
         <v>0</v>
@@ -3782,10 +3782,10 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C62">
         <v>15</v>
@@ -3812,7 +3812,7 @@
         <v>4</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L62" t="b">
         <v>1</v>
@@ -3835,10 +3835,10 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C63">
         <v>15</v>
@@ -3865,7 +3865,7 @@
         <v>4</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L63" t="b">
         <v>0</v>
@@ -3888,10 +3888,10 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C64">
         <v>15</v>
@@ -3918,7 +3918,7 @@
         <v>4</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L64" t="b">
         <v>0</v>
@@ -3941,10 +3941,10 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C65">
         <v>15</v>
@@ -3971,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L65" t="b">
         <v>0</v>
@@ -3994,10 +3994,10 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C66">
         <v>15</v>
@@ -4012,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H66">
         <v>10</v>
@@ -4024,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L66" t="b">
         <v>1</v>
@@ -4047,10 +4047,10 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C67">
         <v>15</v>
@@ -4065,7 +4065,7 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H67">
         <v>10</v>
@@ -4077,7 +4077,7 @@
         <v>4</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L67" t="b">
         <v>0</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C68">
         <v>15</v>
@@ -4118,7 +4118,7 @@
         <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H68">
         <v>10</v>
@@ -4130,7 +4130,7 @@
         <v>4</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L68" t="b">
         <v>0</v>
@@ -4153,10 +4153,10 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C69">
         <v>15</v>
@@ -4171,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H69">
         <v>10</v>
@@ -4183,7 +4183,7 @@
         <v>4</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L69" t="b">
         <v>0</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C70">
         <v>15</v>
@@ -4224,7 +4224,7 @@
         <v>4</v>
       </c>
       <c r="G70" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H70">
         <v>10</v>
@@ -4236,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L70" t="b">
         <v>0</v>
@@ -4259,10 +4259,10 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C71">
         <v>15</v>
@@ -4277,7 +4277,7 @@
         <v>5</v>
       </c>
       <c r="G71" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H71">
         <v>10</v>
@@ -4289,7 +4289,7 @@
         <v>4</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L71" t="b">
         <v>0</v>
@@ -4312,10 +4312,10 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C72">
         <v>15</v>
@@ -4330,7 +4330,7 @@
         <v>6</v>
       </c>
       <c r="G72" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H72">
         <v>10</v>
@@ -4342,7 +4342,7 @@
         <v>4</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L72" t="b">
         <v>1</v>
@@ -4365,10 +4365,10 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C73">
         <v>15</v>
@@ -4383,7 +4383,7 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H73">
         <v>10</v>
@@ -4395,7 +4395,7 @@
         <v>4</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L73" t="b">
         <v>0</v>
@@ -4418,10 +4418,10 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C74">
         <v>15</v>
@@ -4436,7 +4436,7 @@
         <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H74">
         <v>10</v>
@@ -4448,7 +4448,7 @@
         <v>4</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L74" t="b">
         <v>0</v>
@@ -4471,10 +4471,10 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C75">
         <v>15</v>
@@ -4489,7 +4489,7 @@
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H75">
         <v>10</v>
@@ -4501,7 +4501,7 @@
         <v>4</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L75" t="b">
         <v>0</v>
@@ -4524,10 +4524,10 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C76">
         <v>15</v>
@@ -4536,13 +4536,13 @@
         <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H76">
         <v>10</v>
@@ -4554,7 +4554,7 @@
         <v>4</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L76" t="b">
         <v>1</v>
@@ -4577,10 +4577,10 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C77">
         <v>15</v>
@@ -4589,13 +4589,13 @@
         <v>5</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77">
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H77">
         <v>10</v>
@@ -4607,7 +4607,7 @@
         <v>4</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L77" t="b">
         <v>0</v>
@@ -4630,10 +4630,10 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C78">
         <v>15</v>
@@ -4642,13 +4642,13 @@
         <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78">
         <v>2</v>
       </c>
       <c r="G78" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H78">
         <v>10</v>
@@ -4660,7 +4660,7 @@
         <v>4</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L78" t="b">
         <v>0</v>
@@ -4683,10 +4683,10 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C79">
         <v>15</v>
@@ -4695,13 +4695,13 @@
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79">
         <v>3</v>
       </c>
       <c r="G79" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H79">
         <v>10</v>
@@ -4713,7 +4713,7 @@
         <v>4</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L79" t="b">
         <v>0</v>
@@ -4736,10 +4736,10 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C80">
         <v>15</v>
@@ -4748,13 +4748,13 @@
         <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80">
         <v>4</v>
       </c>
       <c r="G80" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H80">
         <v>10</v>
@@ -4766,7 +4766,7 @@
         <v>4</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L80" t="b">
         <v>0</v>
@@ -4789,10 +4789,10 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C81">
         <v>15</v>
@@ -4801,13 +4801,13 @@
         <v>5</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81">
         <v>5</v>
       </c>
       <c r="G81" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H81">
         <v>10</v>
@@ -4819,7 +4819,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L81" t="b">
         <v>0</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C82">
         <v>15</v>
@@ -4854,13 +4854,13 @@
         <v>5</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82">
         <v>6</v>
       </c>
       <c r="G82" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H82">
         <v>10</v>
@@ -4872,7 +4872,7 @@
         <v>4</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L82" t="b">
         <v>1</v>
@@ -4895,10 +4895,10 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C83">
         <v>15</v>
@@ -4907,13 +4907,13 @@
         <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83">
         <v>7</v>
       </c>
       <c r="G83" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H83">
         <v>10</v>
@@ -4925,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L83" t="b">
         <v>0</v>
@@ -4948,10 +4948,10 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C84">
         <v>15</v>
@@ -4960,13 +4960,13 @@
         <v>5</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84">
         <v>8</v>
       </c>
       <c r="G84" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H84">
         <v>10</v>
@@ -4978,7 +4978,7 @@
         <v>4</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L84" t="b">
         <v>0</v>
@@ -5001,10 +5001,10 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C85">
         <v>15</v>
@@ -5013,13 +5013,13 @@
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85">
         <v>9</v>
       </c>
       <c r="G85" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="H85">
         <v>10</v>
@@ -5031,7 +5031,7 @@
         <v>4</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L85" t="b">
         <v>0</v>
@@ -5062,7 +5062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DABA5D-1121-8A47-9E45-66DCFE5B4802}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -5079,10 +5079,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5447,7 +5447,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -5464,7 +5464,7 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -5481,7 +5481,7 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -5498,7 +5498,7 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -5515,7 +5515,7 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -5532,7 +5532,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -5549,7 +5549,7 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -5563,7 +5563,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -5597,7 +5597,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -5648,7 +5648,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -5665,7 +5665,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -5699,7 +5699,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -5750,7 +5750,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -5784,7 +5784,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -5818,7 +5818,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -5835,7 +5835,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -5869,10 +5869,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -5886,10 +5886,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -5903,10 +5903,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -5920,10 +5920,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -5937,10 +5937,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -5954,10 +5954,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>6</v>

</xml_diff>

<commit_message>
add sample_info for dna, add dna id column in metadata for doc and fcm files, duplicate t0 dna samples for each bottle
</commit_message>
<xml_diff>
--- a/Input_Data/week3/ACIDD_Exp_BactAbund.xlsx
+++ b/Input_Data/week3/ACIDD_Exp_BactAbund.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasbaetge/GITHUB/eemb144l/Input_Data/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58C4B1C-C5E9-6643-BD8F-A6F70E5406E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1088BA9-3051-A942-8529-409738496186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18400" yWindow="3440" windowWidth="26840" windowHeight="15940" xr2:uid="{DFE3F779-83E5-5C45-8A1C-F78D6D093241}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="62">
   <si>
     <t>Experiment</t>
   </si>
@@ -169,6 +169,57 @@
   </si>
   <si>
     <t>Ash Leachate</t>
+  </si>
+  <si>
+    <t>DNA_SampleID</t>
+  </si>
+  <si>
+    <t>ASH171-A0_S293</t>
+  </si>
+  <si>
+    <t>ASH171-A6_S295</t>
+  </si>
+  <si>
+    <t>ASH171-B0_S293</t>
+  </si>
+  <si>
+    <t>ASH171-B6_S296</t>
+  </si>
+  <si>
+    <t>ASH171-C0_S294</t>
+  </si>
+  <si>
+    <t>ASH171-C6_S297</t>
+  </si>
+  <si>
+    <t>ASH171-D0_S294</t>
+  </si>
+  <si>
+    <t>ASH171-D6_S298</t>
+  </si>
+  <si>
+    <t>ASH172-A0_S299</t>
+  </si>
+  <si>
+    <t>ASH172-A5_S301</t>
+  </si>
+  <si>
+    <t>ASH172-B0_S299</t>
+  </si>
+  <si>
+    <t>ASH172-B5_S302</t>
+  </si>
+  <si>
+    <t>ASH172-C0_S300</t>
+  </si>
+  <si>
+    <t>ASH172-C5_S303</t>
+  </si>
+  <si>
+    <t>ASH172-D0_S300</t>
+  </si>
+  <si>
+    <t>ASH172-D5_S304</t>
   </si>
 </sst>
 </file>
@@ -176,7 +227,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -223,8 +274,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,15 +590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0444EC-73B7-544C-8786-238F0C09BB54}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:XFD81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +650,11 @@
       <c r="Q1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -652,8 +706,11 @@
       <c r="Q2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -706,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -759,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -812,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -865,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -918,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -970,8 +1027,11 @@
       <c r="Q8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1024,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1183,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1235,8 +1295,11 @@
       <c r="Q13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1395,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1501,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1553,8 +1616,11 @@
       <c r="Q19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1660,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1713,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1766,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1818,8 +1884,11 @@
       <c r="Q24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1978,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2031,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2084,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2136,8 +2205,11 @@
       <c r="Q30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2190,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2243,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2296,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2349,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2401,8 +2473,11 @@
       <c r="Q35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2455,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2508,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2561,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2667,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2719,8 +2794,11 @@
       <c r="Q41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2773,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2879,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2932,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2984,8 +3062,11 @@
       <c r="Q46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -3038,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3091,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -3144,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -3197,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -3250,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -3302,8 +3383,11 @@
       <c r="Q52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -3356,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -3462,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3514,8 +3598,11 @@
       <c r="Q56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -3568,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3621,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -3674,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3727,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3779,8 +3866,11 @@
       <c r="Q61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -3833,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -3886,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3939,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -3992,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -4044,8 +4134,11 @@
       <c r="Q66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -4098,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -4151,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -4204,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -4257,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -4309,8 +4402,11 @@
       <c r="Q71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -4363,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -4416,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -4469,7 +4565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -4522,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -4574,8 +4670,11 @@
       <c r="Q76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4628,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -4681,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -4734,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -4787,7 +4886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -4839,8 +4938,11 @@
       <c r="Q81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -4893,7 +4995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4946,7 +5048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -4999,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>10</v>
       </c>

</xml_diff>